<commit_message>
Updated Reading planner for April
</commit_message>
<xml_diff>
--- a/pdf_upload/ReadingPlan.xlsx
+++ b/pdf_upload/ReadingPlan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="106">
   <si>
     <t>GENESIS 1-2</t>
   </si>
@@ -264,6 +264,84 @@
   </si>
   <si>
     <t>2 SAMUEL 21-24</t>
+  </si>
+  <si>
+    <t>1 KINGS 1-4</t>
+  </si>
+  <si>
+    <t>1 KINGS 5-8</t>
+  </si>
+  <si>
+    <t>1 KINGS 9-11</t>
+  </si>
+  <si>
+    <t>1 KINGS 12-16</t>
+  </si>
+  <si>
+    <t>1 KINGS 17-19</t>
+  </si>
+  <si>
+    <t>1 KINGS 20-22</t>
+  </si>
+  <si>
+    <t>2 KINGS 1-3</t>
+  </si>
+  <si>
+    <t>2 KINGS 4-8</t>
+  </si>
+  <si>
+    <t>2 KINGS 9-12</t>
+  </si>
+  <si>
+    <t>2 KINGS 13-17</t>
+  </si>
+  <si>
+    <t>2 KINGS 18-21</t>
+  </si>
+  <si>
+    <t>2 KINGS 22-25</t>
+  </si>
+  <si>
+    <t>1 CHRONICLES 1-9</t>
+  </si>
+  <si>
+    <t>1 CHRONICLES 10-16</t>
+  </si>
+  <si>
+    <t>1 CHRONICLES 17-21</t>
+  </si>
+  <si>
+    <t>1 CHRONICLES 22-27</t>
+  </si>
+  <si>
+    <t>1 CHRONICLES 28-29</t>
+  </si>
+  <si>
+    <t>2 CHRONICLES 1-5</t>
+  </si>
+  <si>
+    <t>2 CHRONICLES 6-9</t>
+  </si>
+  <si>
+    <t>2 CHRONICLES 10-12</t>
+  </si>
+  <si>
+    <t>2 CHRONICLES 13-16</t>
+  </si>
+  <si>
+    <t>2 CHRONICLES 17-20</t>
+  </si>
+  <si>
+    <t>2 CHRONICLES 21-25</t>
+  </si>
+  <si>
+    <t>2 CHRONICLES 26-28</t>
+  </si>
+  <si>
+    <t>2 CHRONICLES 29-32</t>
+  </si>
+  <si>
+    <t>2 CHRONICLES 33-36</t>
   </si>
 </sst>
 </file>
@@ -586,8 +664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B366"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="B91" sqref="B91"/>
+    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
+      <selection activeCell="B122" sqref="B122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1328,183 +1406,273 @@
       <c r="A92" s="1">
         <v>45017</v>
       </c>
+      <c r="B92" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>45018</v>
       </c>
+      <c r="B93" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>45019</v>
       </c>
+      <c r="B94" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>45020</v>
       </c>
+      <c r="B95" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>45021</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B96" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>45022</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B97" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>45023</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B98" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>45024</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B99" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>45025</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B100" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>45026</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B101" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>45027</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B102" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>45028</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B103" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>45029</v>
       </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B104" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>45030</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B105" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>45031</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B106" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>45032</v>
       </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B107" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>45033</v>
       </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B108" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>45034</v>
       </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B109" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>45035</v>
       </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B110" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>45036</v>
       </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B111" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>45037</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B112" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>45038</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B113" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>45039</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B114" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>45040</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B115" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>45041</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B116" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>45042</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B117" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>45043</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B118" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>45044</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B119" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>45045</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B120" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>45046</v>
       </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B121" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>45047</v>
       </c>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>45048</v>
       </c>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>45049</v>
       </c>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>45050</v>
       </c>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <v>45051</v>
       </c>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>45052</v>
       </c>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
         <v>45053</v>
       </c>

</xml_diff>